<commit_message>
Adicinando as quantidades de acertos
</commit_message>
<xml_diff>
--- a/CHResultadoMicrodados.xlsx
+++ b/CHResultadoMicrodados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>MÁXIMO</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>QUANTIDADE</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,6 +473,9 @@
       <c r="D2" t="n">
         <v>328.4</v>
       </c>
+      <c r="E2" t="n">
+        <v>5066</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -482,6 +490,9 @@
       <c r="D3" t="n">
         <v>353.3</v>
       </c>
+      <c r="E3" t="n">
+        <v>688</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -496,6 +507,9 @@
       <c r="D4" t="n">
         <v>376.9</v>
       </c>
+      <c r="E4" t="n">
+        <v>1472</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -510,6 +524,9 @@
       <c r="D5" t="n">
         <v>399.1</v>
       </c>
+      <c r="E5" t="n">
+        <v>4322</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -524,6 +541,9 @@
       <c r="D6" t="n">
         <v>429.4</v>
       </c>
+      <c r="E6" t="n">
+        <v>11323</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -538,6 +558,9 @@
       <c r="D7" t="n">
         <v>449.2</v>
       </c>
+      <c r="E7" t="n">
+        <v>24621</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -552,6 +575,9 @@
       <c r="D8" t="n">
         <v>471.4</v>
       </c>
+      <c r="E8" t="n">
+        <v>45925</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -566,6 +592,9 @@
       <c r="D9" t="n">
         <v>486.8</v>
       </c>
+      <c r="E9" t="n">
+        <v>73876</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -580,6 +609,9 @@
       <c r="D10" t="n">
         <v>498.5</v>
       </c>
+      <c r="E10" t="n">
+        <v>105679</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -594,6 +626,9 @@
       <c r="D11" t="n">
         <v>514.3</v>
       </c>
+      <c r="E11" t="n">
+        <v>135953</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -608,6 +643,9 @@
       <c r="D12" t="n">
         <v>520.9</v>
       </c>
+      <c r="E12" t="n">
+        <v>159350</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -622,6 +660,9 @@
       <c r="D13" t="n">
         <v>535.6</v>
       </c>
+      <c r="E13" t="n">
+        <v>175123</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -636,6 +677,9 @@
       <c r="D14" t="n">
         <v>544.7</v>
       </c>
+      <c r="E14" t="n">
+        <v>182628</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -650,6 +694,9 @@
       <c r="D15" t="n">
         <v>554.4</v>
       </c>
+      <c r="E15" t="n">
+        <v>179784</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -664,6 +711,9 @@
       <c r="D16" t="n">
         <v>563.2</v>
       </c>
+      <c r="E16" t="n">
+        <v>171240</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -678,6 +728,9 @@
       <c r="D17" t="n">
         <v>576.1</v>
       </c>
+      <c r="E17" t="n">
+        <v>159715</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -692,6 +745,9 @@
       <c r="D18" t="n">
         <v>587.8</v>
       </c>
+      <c r="E18" t="n">
+        <v>145280</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -706,6 +762,9 @@
       <c r="D19" t="n">
         <v>600.1</v>
       </c>
+      <c r="E19" t="n">
+        <v>130238</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -720,6 +779,9 @@
       <c r="D20" t="n">
         <v>605.6</v>
       </c>
+      <c r="E20" t="n">
+        <v>115939</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -734,6 +796,9 @@
       <c r="D21" t="n">
         <v>613.3</v>
       </c>
+      <c r="E21" t="n">
+        <v>102726</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -748,6 +813,9 @@
       <c r="D22" t="n">
         <v>624.4</v>
       </c>
+      <c r="E22" t="n">
+        <v>89889</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -762,6 +830,9 @@
       <c r="D23" t="n">
         <v>631.1</v>
       </c>
+      <c r="E23" t="n">
+        <v>79119</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -776,6 +847,9 @@
       <c r="D24" t="n">
         <v>633.9</v>
       </c>
+      <c r="E24" t="n">
+        <v>69986</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -790,6 +864,9 @@
       <c r="D25" t="n">
         <v>640.5</v>
       </c>
+      <c r="E25" t="n">
+        <v>61556</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -804,6 +881,9 @@
       <c r="D26" t="n">
         <v>647.6</v>
       </c>
+      <c r="E26" t="n">
+        <v>55091</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -818,6 +898,9 @@
       <c r="D27" t="n">
         <v>653.3</v>
       </c>
+      <c r="E27" t="n">
+        <v>48274</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -832,6 +915,9 @@
       <c r="D28" t="n">
         <v>659.6</v>
       </c>
+      <c r="E28" t="n">
+        <v>43156</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -846,6 +932,9 @@
       <c r="D29" t="n">
         <v>665.4</v>
       </c>
+      <c r="E29" t="n">
+        <v>38506</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -860,6 +949,9 @@
       <c r="D30" t="n">
         <v>668.8</v>
       </c>
+      <c r="E30" t="n">
+        <v>34873</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -874,6 +966,9 @@
       <c r="D31" t="n">
         <v>680.4</v>
       </c>
+      <c r="E31" t="n">
+        <v>31073</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -888,6 +983,9 @@
       <c r="D32" t="n">
         <v>686.7</v>
       </c>
+      <c r="E32" t="n">
+        <v>27784</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -902,6 +1000,9 @@
       <c r="D33" t="n">
         <v>694.6</v>
       </c>
+      <c r="E33" t="n">
+        <v>25042</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -916,6 +1017,9 @@
       <c r="D34" t="n">
         <v>700</v>
       </c>
+      <c r="E34" t="n">
+        <v>22536</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -930,6 +1034,9 @@
       <c r="D35" t="n">
         <v>706.5</v>
       </c>
+      <c r="E35" t="n">
+        <v>19737</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -944,6 +1051,9 @@
       <c r="D36" t="n">
         <v>718.4</v>
       </c>
+      <c r="E36" t="n">
+        <v>17555</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -958,6 +1068,9 @@
       <c r="D37" t="n">
         <v>725</v>
       </c>
+      <c r="E37" t="n">
+        <v>15673</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -972,6 +1085,9 @@
       <c r="D38" t="n">
         <v>731.9</v>
       </c>
+      <c r="E38" t="n">
+        <v>13189</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -986,6 +1102,9 @@
       <c r="D39" t="n">
         <v>744</v>
       </c>
+      <c r="E39" t="n">
+        <v>11060</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1000,6 +1119,9 @@
       <c r="D40" t="n">
         <v>756.2</v>
       </c>
+      <c r="E40" t="n">
+        <v>8994</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1014,6 +1136,9 @@
       <c r="D41" t="n">
         <v>767.4</v>
       </c>
+      <c r="E41" t="n">
+        <v>7050</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1028,6 +1153,9 @@
       <c r="D42" t="n">
         <v>783.6</v>
       </c>
+      <c r="E42" t="n">
+        <v>4849</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1042,6 +1170,9 @@
       <c r="D43" t="n">
         <v>794.3</v>
       </c>
+      <c r="E43" t="n">
+        <v>3187</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1056,6 +1187,9 @@
       <c r="D44" t="n">
         <v>809</v>
       </c>
+      <c r="E44" t="n">
+        <v>1821</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1070,6 +1204,9 @@
       <c r="D45" t="n">
         <v>823.4</v>
       </c>
+      <c r="E45" t="n">
+        <v>727</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1084,6 +1221,9 @@
       <c r="D46" t="n">
         <v>844</v>
       </c>
+      <c r="E46" t="n">
+        <v>262</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1097,6 +1237,9 @@
       </c>
       <c r="D47" t="n">
         <v>862.6</v>
+      </c>
+      <c r="E47" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>